<commit_message>
validate bank accounts and make list for browser
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dane\Python\Wlasne\WhiteList\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2323164-C1AD-4A4C-89D4-64417749341C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99381AF0-8E38-432D-91C4-EA23088B7F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49050" yWindow="3240" windowWidth="7380" windowHeight="7320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Numer konta</t>
   </si>
@@ -40,16 +40,25 @@
   </si>
   <si>
     <t>11 1540 1098 2059 0001 1118 0001</t>
+  </si>
+  <si>
+    <t>34 1240 1268 1111 0011 2501 0489</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -358,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +404,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functions for button which opens input or output files
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dane\Python\Wlasne\WhiteList\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34858E5D-3A35-44E6-B291-8902F904950C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F12A9B-FEB5-4FE3-86DB-BA1EC9811D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49050" yWindow="3240" windowWidth="7380" windowHeight="7320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>34 1240 1268 1111 0011 2501 0489</t>
   </si>
   <si>
-    <t>77x1240 1268 1111 0010 6850 0503</t>
+    <t>77 1240 1268 1111 0010 6850 0503</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>